<commit_message>
Finalizacion login y registro de usuario
</commit_message>
<xml_diff>
--- a/Normalizacion.xlsx
+++ b/Normalizacion.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\droid\Desktop\ProyectoColaborativo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ProyectoColaborativo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="79">
   <si>
     <t>jlopeza</t>
   </si>
@@ -246,6 +246,21 @@
   </si>
   <si>
     <t>numReleases</t>
+  </si>
+  <si>
+    <t>Rol</t>
+  </si>
+  <si>
+    <t>idRol</t>
+  </si>
+  <si>
+    <t>Lider</t>
+  </si>
+  <si>
+    <t>Stakeholder</t>
+  </si>
+  <si>
+    <t>Programador</t>
   </si>
 </sst>
 </file>
@@ -277,7 +292,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -332,6 +347,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -360,7 +381,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -376,6 +397,7 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:S65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D37" workbookViewId="0">
-      <selection activeCell="N64" sqref="N64"/>
+    <sheetView tabSelected="1" topLeftCell="D40" workbookViewId="0">
+      <selection activeCell="Q51" sqref="Q51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1505,7 +1527,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>5</v>
       </c>
@@ -1537,7 +1559,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>6</v>
       </c>
@@ -1545,12 +1567,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>57</v>
       </c>
@@ -1570,7 +1592,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="11">
         <v>1</v>
       </c>
@@ -1590,7 +1612,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="11">
         <v>2</v>
       </c>
@@ -1610,12 +1632,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>24</v>
       </c>
@@ -1626,7 +1648,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>25</v>
       </c>
@@ -1672,8 +1694,11 @@
       <c r="Q43" s="7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R43" s="15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
         <v>1</v>
       </c>
@@ -1719,8 +1744,11 @@
       <c r="Q44" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R44" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
         <v>2</v>
       </c>
@@ -1766,8 +1794,11 @@
       <c r="Q45" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R45" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
         <v>3</v>
       </c>
@@ -1792,11 +1823,14 @@
       <c r="Q46" s="7">
         <v>3</v>
       </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R46" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="L47" s="13"/>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>9</v>
       </c>
@@ -2049,6 +2083,9 @@
       <c r="H59" t="s">
         <v>16</v>
       </c>
+      <c r="K59" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="11" t="s">
@@ -2075,6 +2112,12 @@
       <c r="I60" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="K60" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="L60" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
@@ -2101,6 +2144,12 @@
       <c r="I61" s="2" t="s">
         <v>72</v>
       </c>
+      <c r="K61" s="15">
+        <v>1</v>
+      </c>
+      <c r="L61" s="2" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="11">
@@ -2126,6 +2175,12 @@
       </c>
       <c r="I62" s="2" t="s">
         <v>70</v>
+      </c>
+      <c r="K62" s="15">
+        <v>2</v>
+      </c>
+      <c r="L62" s="2" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
@@ -2134,6 +2189,12 @@
       </c>
       <c r="I63" s="2" t="s">
         <v>71</v>
+      </c>
+      <c r="K63" s="15">
+        <v>3</v>
+      </c>
+      <c r="L63" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>